<commit_message>
Update code for Entity
</commit_message>
<xml_diff>
--- a/Function_Design.xlsx
+++ b/Function_Design.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
   <si>
     <t>User story</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>- IsDefault</t>
+  </si>
+  <si>
+    <t>ProductInTransactions</t>
   </si>
 </sst>
 </file>
@@ -509,12 +512,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -544,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -560,6 +575,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,6 +590,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -617,7 +641,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -652,7 +676,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1268,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1280,10 +1304,11 @@
     <col min="4" max="4" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1295,21 +1320,21 @@
         <v>75</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>102</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>135</v>
       </c>
       <c r="G2" s="7"/>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1328,11 +1353,11 @@
         <v>76</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -1351,11 +1376,11 @@
         <v>115</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -1374,11 +1399,11 @@
         <v>82</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -1397,11 +1422,11 @@
         <v>104</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -1420,11 +1445,11 @@
         <v>107</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="6"/>
       <c r="M7" s="5"/>
@@ -1443,11 +1468,11 @@
         <v>109</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
       <c r="M8" s="5"/>
@@ -1485,11 +1510,13 @@
         <v>136</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
       <c r="M10" s="5"/>
@@ -1502,10 +1529,12 @@
       <c r="E11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1518,10 +1547,12 @@
       <c r="C12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1532,21 +1563,21 @@
         <v>76</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="9" t="s">
         <v>113</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="10" t="s">
         <v>138</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1565,11 +1596,11 @@
         <v>76</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1588,11 +1619,11 @@
         <v>139</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1608,11 +1639,11 @@
         <v>82</v>
       </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1652,11 +1683,11 @@
         <v>110</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -1673,11 +1704,11 @@
         <v>114</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1685,18 +1716,18 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
-      <c r="H20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1753,7 +1784,7 @@
       <c r="B27" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="10" t="s">
         <v>117</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -1842,7 +1873,7 @@
       <c r="B37" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="10" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1885,7 +1916,7 @@
       <c r="B43" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="10" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1912,7 +1943,7 @@
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="10" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="3" t="s">

</xml_diff>

<commit_message>
Update code for Fluent  API
</commit_message>
<xml_diff>
--- a/Function_Design.xlsx
+++ b/Function_Design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
   <si>
     <t>User story</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>- Quantity(Số lượng)</t>
+  </si>
+  <si>
+    <t>&lt;-</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,6 +594,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1302,700 +1311,734 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N52"/>
+  <dimension ref="B2:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="2"/>
     <col min="2" max="2" width="28.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="3.28515625" style="2"/>
+    <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="3.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7"/>
+      <c r="F2" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="F3" s="3" t="s">
         <v>76</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="I3" s="5"/>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5"/>
+      <c r="F4" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5"/>
+      <c r="F5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5"/>
+      <c r="F6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5"/>
+      <c r="F7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="6"/>
       <c r="M7" s="5"/>
       <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5"/>
+      <c r="F8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
       <c r="M8" s="5"/>
       <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="6"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O9" s="5"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="9" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="6"/>
       <c r="M10" s="5"/>
       <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O10" s="5"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="D11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" s="5"/>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="5"/>
+      <c r="L11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="3" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="E12" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5"/>
+      <c r="F13" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="5"/>
+      <c r="L13" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="F14" s="3" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="H14" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="5"/>
+      <c r="L14" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="5"/>
+      <c r="F15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="3" t="s">
+      <c r="K15" s="5"/>
+      <c r="L15" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="3" t="s">
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D16" s="5"/>
+      <c r="F16" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="6"/>
+      <c r="H16" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="5"/>
+      <c r="L16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="F17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="F18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="6"/>
+      <c r="H18" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="9" t="s">
+      <c r="K18" s="6"/>
+      <c r="L18" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="6"/>
+      <c r="L19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
-      <c r="F20" s="3" t="s">
+      <c r="C20" s="5"/>
+      <c r="H20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D21" s="11" t="s">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F21" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="C22" s="7"/>
+      <c r="F22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="C23" s="5"/>
+      <c r="F23" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="C24" s="5"/>
+      <c r="F24" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="C25" s="5"/>
+      <c r="F25" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F26" s="3" t="s">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H26" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="C27" s="7"/>
+      <c r="F27" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="5"/>
+      <c r="F28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="C29" s="5"/>
+      <c r="F29" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D30" s="3" t="s">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="C31" s="7"/>
+      <c r="F31" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="C32" s="5"/>
+      <c r="F32" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="C33" s="5"/>
+      <c r="F33" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="C34" s="5"/>
+      <c r="F34" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="C35" s="5"/>
+      <c r="F35" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="C37" s="5"/>
+      <c r="F37" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
-      <c r="D38" s="3" t="s">
+      <c r="C38" s="5"/>
+      <c r="F38" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="C39" s="7"/>
+      <c r="F39" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="C40" s="5"/>
+      <c r="F40" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="C41" s="5"/>
+      <c r="F41" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="C43" s="5"/>
+      <c r="F43" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="C44" s="5"/>
+      <c r="F44" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="C45" s="5"/>
+      <c r="F45" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="6"/>
-      <c r="D46" s="3" t="s">
+      <c r="C46" s="6"/>
+      <c r="F46" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="C47" s="12"/>
+      <c r="F47" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="C48" s="5"/>
+      <c r="F48" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="C49" s="5"/>
+      <c r="F49" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D50" s="3" t="s">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F50" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D51" s="3" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F51" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D52" s="3" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F52" s="3" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>